<commit_message>
Updated files. New Sprint has started!
</commit_message>
<xml_diff>
--- a/Scrum/Scrum board.xlsx
+++ b/Scrum/Scrum board.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\ES\ES_gantProject\Scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Faculdade\3ºano\1º Semestre\ES\1ºfase\ES_gantProject\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBCF88E-8601-4CA1-BB26-FBD832617BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F302CD-BA45-4DF8-8443-B30296F1A959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>Task Description</t>
   </si>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t>1º Sprint</t>
+  </si>
+  <si>
+    <t>2º Sprint</t>
+  </si>
+  <si>
+    <t>1º functionality</t>
+  </si>
+  <si>
+    <t>2º functionality</t>
+  </si>
+  <si>
+    <t>Guilherme          Joana                 Leticia</t>
   </si>
 </sst>
 </file>
@@ -211,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -388,11 +400,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -442,6 +495,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,28 +785,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:H17"/>
+  <dimension ref="B3:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="5" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="3" max="5" width="14.1796875" customWidth="1"/>
+    <col min="7" max="8" width="17.7265625" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" customWidth="1"/>
+    <col min="10" max="10" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>0</v>
       </c>
@@ -757,14 +828,30 @@
       <c r="E6" s="15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="14"/>
       <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -777,8 +864,16 @@
       <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="2:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -791,8 +886,16 @@
       <c r="E9" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -806,7 +909,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -820,7 +923,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
@@ -834,7 +937,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -849,7 +952,7 @@
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -863,7 +966,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -877,7 +980,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -891,7 +994,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
@@ -906,7 +1009,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>

</xml_diff>

<commit_message>
updated scrum board and report
</commit_message>
<xml_diff>
--- a/Scrum/Scrum board.xlsx
+++ b/Scrum/Scrum board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\disnoca\Documents\Universidade\ES\GantProject\ES_gantProject\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF7F01A-E3C5-4F5E-B686-D8CB4A649A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E556B760-8D8A-463B-B80A-48B3DA018534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>Task Description</t>
   </si>
@@ -175,6 +175,29 @@
     <t>Guilherme
 Joana
 Leticia</t>
+  </si>
+  <si>
+    <t>Leticia</t>
+  </si>
+  <si>
+    <t>Samuel
+Joana</t>
+  </si>
+  <si>
+    <t>Guilherme                                                          Samuel
+Joana
+Leticia</t>
+  </si>
+  <si>
+    <t>Guilherme                                        Samuel
+Joana
+Leticia</t>
+  </si>
+  <si>
+    <t>Samuel                                                              Leticia                                                         Guilherme                                                            Joana</t>
+  </si>
+  <si>
+    <t>not done because of reasons explained in the report</t>
   </si>
 </sst>
 </file>
@@ -226,8 +249,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -521,15 +543,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -537,6 +550,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -555,11 +574,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -841,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:T17"/>
+  <dimension ref="B3:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,102 +886,102 @@
     <col min="20" max="20" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="G3" s="26" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="G3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="L3" s="26" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="L3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="Q3" s="26" t="s">
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="Q3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
     </row>
-    <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
+    <row r="5" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="J6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="N6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="24" t="s">
+      <c r="O6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="20" t="s">
+      <c r="Q6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="S6" s="22" t="s">
+      <c r="S6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="24" t="s">
+      <c r="T6" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="25"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="25"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="25"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="25"/>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="24"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="24"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="24"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="24"/>
     </row>
-    <row r="8" spans="2:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -993,11 +1015,17 @@
       <c r="Q8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R8" s="15"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="2"/>
+      <c r="R8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="9" spans="2:20" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:21" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1035,13 +1063,16 @@
       <c r="Q9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R9" s="27" t="s">
+      <c r="R9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="S9" s="14"/>
+      <c r="S9" s="8"/>
       <c r="T9" s="2"/>
+      <c r="U9" s="27" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="10" spans="2:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -1054,20 +1085,20 @@
       <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q10" s="17" t="s">
+      <c r="Q10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="R10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S10" s="8" t="s">
-        <v>16</v>
+      <c r="R10" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="S10" s="25" t="s">
+        <v>47</v>
       </c>
       <c r="T10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -1080,20 +1111,20 @@
       <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q11" s="17" t="s">
+      <c r="Q11" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="R11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S11" s="8" t="s">
-        <v>16</v>
+      <c r="R11" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="S11" s="25" t="s">
+        <v>47</v>
       </c>
       <c r="T11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1106,11 +1137,11 @@
       <c r="E12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q12" s="17" t="s">
+      <c r="Q12" s="14" t="s">
         <v>39</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="S12" s="8" t="s">
         <v>16</v>
@@ -1119,7 +1150,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:21" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -1133,19 +1164,21 @@
         <v>24</v>
       </c>
       <c r="H13" s="10"/>
-      <c r="I13" s="19"/>
-      <c r="Q13" s="18" t="s">
+      <c r="I13" s="16"/>
+      <c r="Q13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="R13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="S13" s="16"/>
+      <c r="R13" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="S13" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="T13" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1159,7 +1192,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -1173,7 +1206,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -1203,26 +1236,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="Q3:T3"/>
     <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="R6:R7"/>
     <mergeCell ref="S6:S7"/>
     <mergeCell ref="T6:T7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="L3:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>